<commit_message>
Test cases was failing it is fixed now
</commit_message>
<xml_diff>
--- a/keywords/TC001.xlsx
+++ b/keywords/TC001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="11550" windowHeight="2160"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11310" windowHeight="2220"/>
   </bookViews>
   <sheets>
     <sheet name="TC001" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Locator</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>clickById</t>
+  </si>
+  <si>
+    <t>XXXXXX</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -471,7 +474,9 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
@@ -480,7 +485,9 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
@@ -492,7 +499,11 @@
       <c r="C4" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="karim_94123@yahoo.co.in"/>
+    <hyperlink ref="C3" r:id="rId2" display="P@ssw0rdL"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>